<commit_message>
Updated to include some tests
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>accuracy(%)</t>
   </si>
@@ -35,19 +35,34 @@
     <t>k</t>
   </si>
   <si>
-    <t>50/50</t>
+    <t>accuracy</t>
   </si>
   <si>
-    <t>90/10 (1.4.3)</t>
+    <t>time</t>
   </si>
   <si>
-    <t>90/10 (1.4.4)</t>
+    <t>mean</t>
   </si>
   <si>
-    <t>sig=0.55</t>
+    <t>SD</t>
   </si>
   <si>
-    <t>sig=0.75</t>
+    <t>(1.4.3) 90/10 split, 10 runs</t>
+  </si>
+  <si>
+    <t>(1.4.4)90/10, gaussian sig=0.55</t>
+  </si>
+  <si>
+    <t>(1.4.4)90/10, gaussian sig=0.75</t>
+  </si>
+  <si>
+    <t>many persons, 90/10 split</t>
+  </si>
+  <si>
+    <t>50/50 split</t>
+  </si>
+  <si>
+    <t>k testing</t>
   </si>
 </sst>
 </file>
@@ -125,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -135,6 +150,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,13 +476,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.44140625" customWidth="1"/>
     <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
@@ -475,23 +500,23 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="K1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="O1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
@@ -503,6 +528,9 @@
       <c r="C2" s="1">
         <v>94.95</v>
       </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
       <c r="G2" s="2">
         <v>1</v>
       </c>
@@ -883,6 +911,9 @@
       <c r="C12" s="1">
         <v>91.5</v>
       </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
       <c r="H12">
         <f>AVERAGE(H2:H11)</f>
         <v>59.580999999999996</v>
@@ -891,6 +922,9 @@
         <f>AVERAGE(I2:I11)</f>
         <v>91.2</v>
       </c>
+      <c r="K12" t="s">
+        <v>5</v>
+      </c>
       <c r="L12">
         <f>AVERAGE(L2:L11)</f>
         <v>61.185000000000002</v>
@@ -899,8 +933,22 @@
         <f>AVERAGE(M2:M11)</f>
         <v>95.9</v>
       </c>
+      <c r="O12" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12">
+        <f>AVERAGE(P2:P11)</f>
+        <v>58.864999999999995</v>
+      </c>
+      <c r="Q12">
+        <f>AVERAGE(Q2:Q11)</f>
+        <v>95.9</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>6</v>
+      </c>
       <c r="H13">
         <f>STDEV(H2:H12)</f>
         <v>0.52605037781566089</v>
@@ -909,6 +957,9 @@
         <f>STDEV(I2:I12)</f>
         <v>0.94074438611133893</v>
       </c>
+      <c r="K13" t="s">
+        <v>6</v>
+      </c>
       <c r="L13">
         <f>STDEV(L2:L12)</f>
         <v>4.9271294888606283</v>
@@ -917,6 +968,17 @@
         <f>STDEV(M2:M12)</f>
         <v>0.62449979983983983</v>
       </c>
+      <c r="O13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P13">
+        <f>STDEV(P2:P12)</f>
+        <v>1.0949543369474366</v>
+      </c>
+      <c r="Q13">
+        <f>STDEV(Q2:Q12)</f>
+        <v>0.62449979983983983</v>
+      </c>
     </row>
     <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
@@ -948,6 +1010,11 @@
       <c r="I15" s="1">
         <v>90.25</v>
       </c>
+      <c r="K15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
@@ -968,8 +1035,14 @@
       <c r="I16" s="3">
         <v>91.75</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -988,8 +1061,17 @@
       <c r="I17" s="1">
         <v>90</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>93.15</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0.72140000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -1008,8 +1090,17 @@
       <c r="I18" s="3">
         <v>90.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="3">
+        <v>8563.25</v>
+      </c>
+      <c r="M18" s="5">
+        <v>42.113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -1029,7 +1120,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>16</v>
       </c>
@@ -1049,7 +1140,7 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>17</v>
       </c>
@@ -1069,7 +1160,7 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>18</v>
       </c>
@@ -1089,7 +1180,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>19</v>
       </c>
@@ -1109,7 +1200,7 @@
         <v>92.75</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>20</v>
       </c>
@@ -1128,7 +1219,7 @@
         <v>91.194444444444443</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>21</v>
       </c>
@@ -1147,7 +1238,7 @@
         <v>0.9914760165319304</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>22</v>
       </c>
@@ -1158,7 +1249,7 @@
         <v>91.45</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>23</v>
       </c>
@@ -1169,7 +1260,7 @@
         <v>91.3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>24</v>
       </c>
@@ -1180,7 +1271,7 @@
         <v>90.8</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>25</v>
       </c>
@@ -1191,7 +1282,7 @@
         <v>90.9</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>26</v>
       </c>
@@ -1202,7 +1293,7 @@
         <v>90.65</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>27</v>
       </c>
@@ -1213,7 +1304,7 @@
         <v>90.4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>28</v>
       </c>
@@ -1809,6 +1900,12 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="K15:M15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated 20:38 for 1.4.5
situation 1: all people combined then shuffled
situation 2: training set is 1 group of people, testing set is another
</commit_message>
<xml_diff>
--- a/stats.xlsx
+++ b/stats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>accuracy(%)</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>k=68</t>
+  </si>
+  <si>
+    <t>setup 1</t>
+  </si>
+  <si>
+    <t>setup 2</t>
   </si>
 </sst>
 </file>
@@ -494,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,11 +587,8 @@
       <c r="Q2" s="1">
         <v>96</v>
       </c>
-      <c r="T2" t="s">
-        <v>5</v>
-      </c>
-      <c r="U2" t="s">
-        <v>6</v>
+      <c r="S2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -625,14 +628,11 @@
       <c r="Q3" s="3">
         <v>96</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="T3" s="1">
-        <v>93.15</v>
-      </c>
-      <c r="U3" s="4">
-        <v>0.72140000000000004</v>
+      <c r="T3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -673,13 +673,13 @@
         <v>96</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T4" s="3">
-        <v>8563.25</v>
-      </c>
-      <c r="U4" s="5">
-        <v>42.113</v>
+        <v>3</v>
+      </c>
+      <c r="T4" s="1">
+        <v>93.15</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0.72140000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -719,6 +719,15 @@
       <c r="Q5" s="3">
         <v>94.75</v>
       </c>
+      <c r="S5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" s="3">
+        <v>8563.25</v>
+      </c>
+      <c r="U5" s="5">
+        <v>42.113</v>
+      </c>
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
@@ -795,6 +804,9 @@
       <c r="Q7" s="3">
         <v>97</v>
       </c>
+      <c r="S7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
@@ -833,6 +845,12 @@
       <c r="Q8" s="1">
         <v>96.5</v>
       </c>
+      <c r="T8" t="s">
+        <v>5</v>
+      </c>
+      <c r="U8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
@@ -871,6 +889,15 @@
       <c r="Q9" s="3">
         <v>96.25</v>
       </c>
+      <c r="S9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" s="1">
+        <v>85.375</v>
+      </c>
+      <c r="U9">
+        <v>0.91220000000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
@@ -908,6 +935,15 @@
       </c>
       <c r="Q10" s="1">
         <v>96</v>
+      </c>
+      <c r="S10" t="s">
+        <v>4</v>
+      </c>
+      <c r="T10" s="1">
+        <v>9736.0499999999993</v>
+      </c>
+      <c r="U10" s="4">
+        <v>53.585999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>